<commit_message>
Remove extraneous app_id from demos and otherwise clarify them
</commit_message>
<xml_diff>
--- a/examples/demo-registrations.xlsx
+++ b/examples/demo-registrations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Data Source</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -101,31 +101,17 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>app_id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>xmlns.exact</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>http://openrosa.org/formdesigner/dd3190c7dd7e9e7d469a9705709f2f6b4e27f1d8</t>
-  </si>
-  <si>
-    <t>YOUR_APP_ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -508,7 +494,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -551,8 +537,8 @@
       <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>23</v>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -562,12 +548,6 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
@@ -610,10 +590,9 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>